<commit_message>
updated files to conform to standard
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_2477.xlsx
+++ b/bioSample/bioSample_2477.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1F5188-6E7E-BC48-89E8-57F860923ACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C961B52-CE27-074E-AB74-EE1E0D2261C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>